<commit_message>
many changes and almost ready for first release
</commit_message>
<xml_diff>
--- a/merged_for_angular.xlsx
+++ b/merged_for_angular.xlsx
@@ -14,141 +14,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>aver</t>
   </si>
   <si>
-    <t>0.750</t>
-  </si>
-  <si>
-    <t>1.500</t>
-  </si>
-  <si>
-    <t>2.500</t>
-  </si>
-  <si>
-    <t>3.500</t>
-  </si>
-  <si>
-    <t>4.500</t>
-  </si>
-  <si>
-    <t>5.500</t>
-  </si>
-  <si>
-    <t>6.500</t>
-  </si>
-  <si>
-    <t>7.500</t>
-  </si>
-  <si>
-    <t>8.500</t>
-  </si>
-  <si>
-    <t>9.500</t>
-  </si>
-  <si>
-    <t>10.500</t>
-  </si>
-  <si>
-    <t>11.500</t>
-  </si>
-  <si>
-    <t>12.500</t>
-  </si>
-  <si>
-    <t>13.500</t>
-  </si>
-  <si>
-    <t>0.750_1</t>
-  </si>
-  <si>
-    <t>1.500_2</t>
-  </si>
-  <si>
-    <t>2.500_2</t>
-  </si>
-  <si>
-    <t>3.500_2</t>
-  </si>
-  <si>
-    <t>4.500_1</t>
-  </si>
-  <si>
-    <t>5.500_1</t>
-  </si>
-  <si>
-    <t>6.500_1</t>
-  </si>
-  <si>
-    <t>7.500_1</t>
-  </si>
-  <si>
-    <t>8.500_1</t>
-  </si>
-  <si>
-    <t>9.500_1</t>
-  </si>
-  <si>
-    <t>10.500_1</t>
-  </si>
-  <si>
-    <t>11.500_1</t>
-  </si>
-  <si>
-    <t>12.500_1</t>
-  </si>
-  <si>
-    <t>13.500_1</t>
-  </si>
-  <si>
-    <t>0.750_2</t>
-  </si>
-  <si>
-    <t>1.500_4</t>
-  </si>
-  <si>
-    <t>2.500_4</t>
-  </si>
-  <si>
-    <t>3.500_4</t>
-  </si>
-  <si>
-    <t>4.500_2</t>
-  </si>
-  <si>
-    <t>5.500_2</t>
-  </si>
-  <si>
-    <t>6.500_2</t>
-  </si>
-  <si>
-    <t>7.500_2</t>
-  </si>
-  <si>
-    <t>8.500_2</t>
-  </si>
-  <si>
-    <t>9.500_2</t>
-  </si>
-  <si>
-    <t>10.500_2</t>
-  </si>
-  <si>
-    <t>11.500_2</t>
-  </si>
-  <si>
-    <t>12.500_2</t>
-  </si>
-  <si>
-    <t>13.500_2</t>
+    <t>1.000</t>
+  </si>
+  <si>
+    <t>2.000</t>
+  </si>
+  <si>
+    <t>3.000</t>
+  </si>
+  <si>
+    <t>4.000</t>
+  </si>
+  <si>
+    <t>5.000</t>
+  </si>
+  <si>
+    <t>6.000</t>
+  </si>
+  <si>
+    <t>7.000</t>
+  </si>
+  <si>
+    <t>8.000</t>
+  </si>
+  <si>
+    <t>9.000</t>
+  </si>
+  <si>
+    <t>10.000</t>
+  </si>
+  <si>
+    <t>11.000</t>
+  </si>
+  <si>
+    <t>12.000</t>
+  </si>
+  <si>
+    <t>13.000</t>
+  </si>
+  <si>
+    <t>14.000</t>
+  </si>
+  <si>
+    <t>1.000_2</t>
+  </si>
+  <si>
+    <t>2.000_2</t>
+  </si>
+  <si>
+    <t>3.000_2</t>
+  </si>
+  <si>
+    <t>4.000_2</t>
+  </si>
+  <si>
+    <t>5.000_1</t>
+  </si>
+  <si>
+    <t>6.000_1</t>
+  </si>
+  <si>
+    <t>7.000_1</t>
+  </si>
+  <si>
+    <t>8.000_1</t>
+  </si>
+  <si>
+    <t>9.000_1</t>
+  </si>
+  <si>
+    <t>10.000_1</t>
+  </si>
+  <si>
+    <t>11.000_1</t>
+  </si>
+  <si>
+    <t>12.000_1</t>
+  </si>
+  <si>
+    <t>13.000_1</t>
+  </si>
+  <si>
+    <t>14.000_1</t>
+  </si>
+  <si>
+    <t>1.000_4</t>
+  </si>
+  <si>
+    <t>2.000_4</t>
+  </si>
+  <si>
+    <t>3.000_4</t>
+  </si>
+  <si>
+    <t>4.000_4</t>
+  </si>
+  <si>
+    <t>5.000_2</t>
+  </si>
+  <si>
+    <t>6.000_2</t>
+  </si>
+  <si>
+    <t>7.000_2</t>
+  </si>
+  <si>
+    <t>8.000_2</t>
+  </si>
+  <si>
+    <t>9.000_2</t>
+  </si>
+  <si>
+    <t>10.000_2</t>
+  </si>
+  <si>
+    <t>11.000_2</t>
+  </si>
+  <si>
+    <t>12.000_2</t>
+  </si>
+  <si>
+    <t>13.000_2</t>
+  </si>
+  <si>
+    <t>14.000_2</t>
   </si>
 </sst>
 </file>
@@ -506,13 +500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT11"/>
+  <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:46">
+    <row r="1" spans="1:44">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,109 +636,103 @@
       <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:44">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>0.00023746</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>0.0005182</v>
       </c>
       <c r="E2">
-        <v>5028700000</v>
+        <v>0.0007431</v>
       </c>
       <c r="F2">
-        <v>10278000000</v>
+        <v>0.0010526</v>
       </c>
       <c r="G2">
-        <v>16859000000</v>
+        <v>0.0012545</v>
       </c>
       <c r="H2">
-        <v>24078000000</v>
+        <v>0.0012391</v>
       </c>
       <c r="I2">
-        <v>31037000000</v>
+        <v>0.0012243</v>
       </c>
       <c r="J2">
-        <v>33884000000</v>
+        <v>0.0011071</v>
       </c>
       <c r="K2">
-        <v>33049000000</v>
+        <v>0.0009872699999999999</v>
       </c>
       <c r="L2">
-        <v>31240000000</v>
+        <v>0.0008913700000000001</v>
       </c>
       <c r="M2">
-        <v>27103000000</v>
+        <v>0.0008273</v>
       </c>
       <c r="N2">
-        <v>24344000000</v>
+        <v>0.0005882800000000001</v>
       </c>
       <c r="O2">
-        <v>24126000000</v>
+        <v>0.00030734</v>
       </c>
       <c r="P2">
-        <v>21383000000</v>
+        <v>0.00021956</v>
       </c>
       <c r="Q2">
-        <v>12197000000</v>
+        <v>0.00023746</v>
       </c>
       <c r="R2">
-        <v>4299900000</v>
+        <v>0.0005182</v>
       </c>
       <c r="S2">
-        <v>5028700000</v>
+        <v>0.0007431</v>
       </c>
       <c r="T2">
-        <v>10278000000</v>
+        <v>0.0010526</v>
       </c>
       <c r="U2">
-        <v>16859000000</v>
+        <v>0.0012545</v>
       </c>
       <c r="V2">
-        <v>24078000000</v>
+        <v>0.0012391</v>
       </c>
       <c r="W2">
-        <v>31037000000</v>
+        <v>0.0012243</v>
       </c>
       <c r="X2">
-        <v>33884000000</v>
+        <v>0.0011071</v>
       </c>
       <c r="Y2">
-        <v>33049000000</v>
+        <v>0.0009872699999999999</v>
       </c>
       <c r="Z2">
-        <v>31240000000</v>
+        <v>0.0008913700000000001</v>
       </c>
       <c r="AA2">
-        <v>27103000000</v>
+        <v>0.0008273</v>
       </c>
       <c r="AB2">
-        <v>24344000000</v>
+        <v>0.0005882800000000001</v>
       </c>
       <c r="AC2">
-        <v>24126000000</v>
+        <v>0.00030734</v>
       </c>
       <c r="AD2">
-        <v>21383000000</v>
+        <v>0.00021956</v>
       </c>
       <c r="AE2">
-        <v>12197000000</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>4299900000</v>
+        <v>0</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -782,109 +770,103 @@
       <c r="AR2">
         <v>0</v>
       </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:44">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>0.00020948</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>0.00044238</v>
       </c>
       <c r="E3">
-        <v>4895800000</v>
+        <v>0.00060517</v>
       </c>
       <c r="F3">
-        <v>9436500000</v>
+        <v>0.00081169</v>
       </c>
       <c r="G3">
-        <v>15109000000</v>
+        <v>0.00092521</v>
       </c>
       <c r="H3">
-        <v>19872000000</v>
+        <v>0.00089567</v>
       </c>
       <c r="I3">
-        <v>24963000000</v>
+        <v>0.00087308</v>
       </c>
       <c r="J3">
-        <v>25501000000</v>
+        <v>0.00078957</v>
       </c>
       <c r="K3">
-        <v>24466000000</v>
+        <v>0.00070853</v>
       </c>
       <c r="L3">
-        <v>22748000000</v>
+        <v>0.00065494</v>
       </c>
       <c r="M3">
-        <v>20167000000</v>
+        <v>0.00061175</v>
       </c>
       <c r="N3">
-        <v>19041000000</v>
+        <v>0.00044355</v>
       </c>
       <c r="O3">
-        <v>17948000000</v>
+        <v>0.00024928</v>
       </c>
       <c r="P3">
-        <v>16495000000</v>
+        <v>0.00019193</v>
       </c>
       <c r="Q3">
-        <v>10311000000</v>
+        <v>0.00020948</v>
       </c>
       <c r="R3">
-        <v>6516000000</v>
+        <v>0.00044238</v>
       </c>
       <c r="S3">
-        <v>4895800000</v>
+        <v>0.00060516</v>
       </c>
       <c r="T3">
-        <v>9436100000</v>
+        <v>0.0008117000000000001</v>
       </c>
       <c r="U3">
-        <v>15109000000</v>
+        <v>0.00092519</v>
       </c>
       <c r="V3">
-        <v>19872000000</v>
+        <v>0.00089567</v>
       </c>
       <c r="W3">
-        <v>24964000000</v>
+        <v>0.00087308</v>
       </c>
       <c r="X3">
-        <v>25501000000</v>
+        <v>0.00078958</v>
       </c>
       <c r="Y3">
-        <v>24466000000</v>
+        <v>0.00070853</v>
       </c>
       <c r="Z3">
-        <v>22748000000</v>
+        <v>0.00065494</v>
       </c>
       <c r="AA3">
-        <v>20167000000</v>
+        <v>0.00061175</v>
       </c>
       <c r="AB3">
-        <v>19041000000</v>
+        <v>0.00044355</v>
       </c>
       <c r="AC3">
-        <v>17948000000</v>
+        <v>0.00024928</v>
       </c>
       <c r="AD3">
-        <v>16495000000</v>
+        <v>0.00019193</v>
       </c>
       <c r="AE3">
-        <v>10311000000</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>6516000000</v>
+        <v>0</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -922,109 +904,103 @@
       <c r="AR3">
         <v>0</v>
       </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:44">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>0.00018186</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>0.00037051</v>
       </c>
       <c r="E4">
-        <v>4408900000</v>
+        <v>0.00047729</v>
       </c>
       <c r="F4">
-        <v>8128600000</v>
+        <v>0.00060093</v>
       </c>
       <c r="G4">
-        <v>12324000000</v>
+        <v>0.00065909</v>
       </c>
       <c r="H4">
-        <v>15020000000</v>
+        <v>0.00062666</v>
       </c>
       <c r="I4">
-        <v>17761000000</v>
+        <v>0.00059077</v>
       </c>
       <c r="J4">
-        <v>17080000000</v>
+        <v>0.00053893</v>
       </c>
       <c r="K4">
-        <v>16206000000</v>
+        <v>0.00049183</v>
       </c>
       <c r="L4">
-        <v>14961000000</v>
+        <v>0.0004631</v>
       </c>
       <c r="M4">
-        <v>13411000000</v>
+        <v>0.00042647</v>
       </c>
       <c r="N4">
-        <v>13202000000</v>
+        <v>0.00031464</v>
       </c>
       <c r="O4">
-        <v>13515000000</v>
+        <v>0.0001958</v>
       </c>
       <c r="P4">
-        <v>11894000000</v>
+        <v>0.00015298</v>
       </c>
       <c r="Q4">
-        <v>8844600000</v>
+        <v>0.00018186</v>
       </c>
       <c r="R4">
-        <v>7660900000</v>
+        <v>0.00037051</v>
       </c>
       <c r="S4">
-        <v>4408700000</v>
+        <v>0.00047729</v>
       </c>
       <c r="T4">
-        <v>8128800000</v>
+        <v>0.00060093</v>
       </c>
       <c r="U4">
-        <v>12324000000</v>
+        <v>0.00065909</v>
       </c>
       <c r="V4">
-        <v>15019000000</v>
+        <v>0.00062666</v>
       </c>
       <c r="W4">
-        <v>17760000000</v>
+        <v>0.00059077</v>
       </c>
       <c r="X4">
-        <v>17080000000</v>
+        <v>0.00053892</v>
       </c>
       <c r="Y4">
-        <v>16206000000</v>
+        <v>0.00049183</v>
       </c>
       <c r="Z4">
-        <v>14961000000</v>
+        <v>0.0004631</v>
       </c>
       <c r="AA4">
-        <v>13411000000</v>
+        <v>0.00042647</v>
       </c>
       <c r="AB4">
-        <v>13202000000</v>
+        <v>0.00031464</v>
       </c>
       <c r="AC4">
-        <v>13515000000</v>
+        <v>0.0001958</v>
       </c>
       <c r="AD4">
-        <v>11894000000</v>
+        <v>0.00015297</v>
       </c>
       <c r="AE4">
-        <v>8844600000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
-        <v>7660900000</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1062,109 +1038,103 @@
       <c r="AR4">
         <v>0</v>
       </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:44">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>0.0001585</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>0.00031005</v>
       </c>
       <c r="E5">
-        <v>3849000000</v>
+        <v>0.00037852</v>
       </c>
       <c r="F5">
-        <v>6905100000</v>
+        <v>0.00045265</v>
       </c>
       <c r="G5">
-        <v>9559800000</v>
+        <v>0.00046896</v>
       </c>
       <c r="H5">
-        <v>11050000000</v>
+        <v>0.00043448</v>
       </c>
       <c r="I5">
-        <v>12150000000</v>
+        <v>0.00040217</v>
       </c>
       <c r="J5">
-        <v>11202000000</v>
+        <v>0.0003643</v>
       </c>
       <c r="K5">
-        <v>10227000000</v>
+        <v>0.00034308</v>
       </c>
       <c r="L5">
-        <v>9258400000</v>
+        <v>0.00033028</v>
       </c>
       <c r="M5">
-        <v>8331300000</v>
+        <v>0.0003013</v>
       </c>
       <c r="N5">
-        <v>8932300000</v>
+        <v>0.00022928</v>
       </c>
       <c r="O5">
-        <v>8787700000</v>
+        <v>0.00015223</v>
       </c>
       <c r="P5">
-        <v>7577100000</v>
+        <v>0.00012543</v>
       </c>
       <c r="Q5">
-        <v>6127500000</v>
+        <v>0.00015849</v>
       </c>
       <c r="R5">
-        <v>5714100000</v>
+        <v>0.00031005</v>
       </c>
       <c r="S5">
-        <v>3849000000</v>
+        <v>0.00037852</v>
       </c>
       <c r="T5">
-        <v>6904800000</v>
+        <v>0.00045264</v>
       </c>
       <c r="U5">
-        <v>9559500000</v>
+        <v>0.00046894</v>
       </c>
       <c r="V5">
-        <v>11050000000</v>
+        <v>0.00043448</v>
       </c>
       <c r="W5">
-        <v>12149000000</v>
+        <v>0.00040217</v>
       </c>
       <c r="X5">
-        <v>11202000000</v>
+        <v>0.0003643</v>
       </c>
       <c r="Y5">
-        <v>10227000000</v>
+        <v>0.00034308</v>
       </c>
       <c r="Z5">
-        <v>9258400000</v>
+        <v>0.00033027</v>
       </c>
       <c r="AA5">
-        <v>8331300000</v>
+        <v>0.0003013</v>
       </c>
       <c r="AB5">
-        <v>8932300000</v>
+        <v>0.00022928</v>
       </c>
       <c r="AC5">
-        <v>8787700000</v>
+        <v>0.00015223</v>
       </c>
       <c r="AD5">
-        <v>7577100000</v>
+        <v>0.00012544</v>
       </c>
       <c r="AE5">
-        <v>6127500000</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <v>5715400000</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <v>0</v>
@@ -1202,109 +1172,103 @@
       <c r="AR5">
         <v>0</v>
       </c>
-      <c r="AS5">
-        <v>0</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:44">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>0.00013797</v>
       </c>
       <c r="D6">
-        <v>36</v>
+        <v>0.00025871</v>
       </c>
       <c r="E6">
-        <v>3379300000</v>
+        <v>0.00029767</v>
       </c>
       <c r="F6">
-        <v>5767800000</v>
+        <v>0.00033718</v>
       </c>
       <c r="G6">
-        <v>7492500000</v>
+        <v>0.00033147</v>
       </c>
       <c r="H6">
-        <v>8272600000</v>
+        <v>0.00030098</v>
       </c>
       <c r="I6">
-        <v>8208700000</v>
+        <v>0.00027151</v>
       </c>
       <c r="J6">
-        <v>7376800000</v>
+        <v>0.00024822</v>
       </c>
       <c r="K6">
-        <v>6521000000</v>
+        <v>0.00023607</v>
       </c>
       <c r="L6">
-        <v>5578200000</v>
+        <v>0.0002328</v>
       </c>
       <c r="M6">
-        <v>5384600000</v>
+        <v>0.00021001</v>
       </c>
       <c r="N6">
-        <v>5694500000</v>
+        <v>0.00016458</v>
       </c>
       <c r="O6">
-        <v>5453700000</v>
+        <v>0.0001176</v>
       </c>
       <c r="P6">
-        <v>4339400000</v>
+        <v>0.00010149</v>
       </c>
       <c r="Q6">
-        <v>3383300000</v>
+        <v>0.00013797</v>
       </c>
       <c r="R6">
-        <v>3061200000</v>
+        <v>0.00025871</v>
       </c>
       <c r="S6">
-        <v>3379300000</v>
+        <v>0.00029767</v>
       </c>
       <c r="T6">
-        <v>5768000000</v>
+        <v>0.00033718</v>
       </c>
       <c r="U6">
-        <v>7492500000</v>
+        <v>0.00033147</v>
       </c>
       <c r="V6">
-        <v>8272600000</v>
+        <v>0.00030098</v>
       </c>
       <c r="W6">
-        <v>8208700000</v>
+        <v>0.00027151</v>
       </c>
       <c r="X6">
-        <v>7376800000</v>
+        <v>0.00024822</v>
       </c>
       <c r="Y6">
-        <v>6521000000</v>
+        <v>0.00023607</v>
       </c>
       <c r="Z6">
-        <v>5578200000</v>
+        <v>0.0002328</v>
       </c>
       <c r="AA6">
-        <v>5384600000</v>
+        <v>0.00020999</v>
       </c>
       <c r="AB6">
-        <v>5694500000</v>
+        <v>0.00016458</v>
       </c>
       <c r="AC6">
-        <v>5453700000</v>
+        <v>0.0001176</v>
       </c>
       <c r="AD6">
-        <v>4339400000</v>
+        <v>0.00010149</v>
       </c>
       <c r="AE6">
-        <v>3383300000</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <v>3061200000</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -1342,109 +1306,103 @@
       <c r="AR6">
         <v>0</v>
       </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:44">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>48</v>
+        <v>0.00012034</v>
       </c>
       <c r="D7">
-        <v>44</v>
+        <v>0.00021537</v>
       </c>
       <c r="E7">
-        <v>2860400000</v>
+        <v>0.0002349</v>
       </c>
       <c r="F7">
-        <v>4854500000</v>
+        <v>0.00025191</v>
       </c>
       <c r="G7">
-        <v>6059600000</v>
+        <v>0.00023438</v>
       </c>
       <c r="H7">
-        <v>6223700000</v>
+        <v>0.00020923</v>
       </c>
       <c r="I7">
-        <v>5833100000</v>
+        <v>0.0001846</v>
       </c>
       <c r="J7">
-        <v>5205000000</v>
+        <v>0.00016819</v>
       </c>
       <c r="K7">
-        <v>4337100000</v>
+        <v>0.00016373</v>
       </c>
       <c r="L7">
-        <v>3655700000</v>
+        <v>0.00016259</v>
       </c>
       <c r="M7">
-        <v>3496400000</v>
+        <v>0.0001478</v>
       </c>
       <c r="N7">
-        <v>3641400000</v>
+        <v>0.00011528</v>
       </c>
       <c r="O7">
-        <v>3272600000</v>
+        <v>9.5506E-05</v>
       </c>
       <c r="P7">
-        <v>2554900000</v>
+        <v>8.5123E-05</v>
       </c>
       <c r="Q7">
-        <v>1683100000</v>
+        <v>0.00012033</v>
       </c>
       <c r="R7">
-        <v>1412400000</v>
+        <v>0.00021537</v>
       </c>
       <c r="S7">
-        <v>2860400000</v>
+        <v>0.0002349</v>
       </c>
       <c r="T7">
-        <v>4854700000</v>
+        <v>0.0002519</v>
       </c>
       <c r="U7">
-        <v>6059600000</v>
+        <v>0.00023438</v>
       </c>
       <c r="V7">
-        <v>6223900000</v>
+        <v>0.00020923</v>
       </c>
       <c r="W7">
-        <v>5833400000</v>
+        <v>0.0001846</v>
       </c>
       <c r="X7">
-        <v>5205000000</v>
+        <v>0.00016819</v>
       </c>
       <c r="Y7">
-        <v>4337100000</v>
+        <v>0.00016373</v>
       </c>
       <c r="Z7">
-        <v>3655700000</v>
+        <v>0.00016259</v>
       </c>
       <c r="AA7">
-        <v>3496400000</v>
+        <v>0.0001478</v>
       </c>
       <c r="AB7">
-        <v>3641400000</v>
+        <v>0.00011528</v>
       </c>
       <c r="AC7">
-        <v>3272600000</v>
+        <v>9.5506E-05</v>
       </c>
       <c r="AD7">
-        <v>2554900000</v>
+        <v>8.5123E-05</v>
       </c>
       <c r="AE7">
-        <v>1683100000</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <v>1412400000</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -1482,109 +1440,103 @@
       <c r="AR7">
         <v>0</v>
       </c>
-      <c r="AS7">
-        <v>0</v>
-      </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:44">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C8">
-        <v>56</v>
+        <v>0.00010454</v>
       </c>
       <c r="D8">
-        <v>52</v>
+        <v>0.00017982</v>
       </c>
       <c r="E8">
-        <v>2449000000</v>
+        <v>0.00018491</v>
       </c>
       <c r="F8">
-        <v>4106300000</v>
+        <v>0.00018653</v>
       </c>
       <c r="G8">
-        <v>4841500000</v>
+        <v>0.00016712</v>
       </c>
       <c r="H8">
-        <v>4833300000</v>
+        <v>0.00014458</v>
       </c>
       <c r="I8">
-        <v>4264800000</v>
+        <v>0.00012603</v>
       </c>
       <c r="J8">
-        <v>3628100000</v>
+        <v>0.00011443</v>
       </c>
       <c r="K8">
-        <v>3088100000</v>
+        <v>0.00011519</v>
       </c>
       <c r="L8">
-        <v>2634100000</v>
+        <v>0.00011466</v>
       </c>
       <c r="M8">
-        <v>2527200000</v>
+        <v>0.00010373</v>
       </c>
       <c r="N8">
-        <v>2484900000</v>
+        <v>8.258399999999999E-05</v>
       </c>
       <c r="O8">
-        <v>2177100000</v>
+        <v>7.425200000000001E-05</v>
       </c>
       <c r="P8">
-        <v>1539500000</v>
+        <v>6.8965E-05</v>
       </c>
       <c r="Q8">
-        <v>1133300000</v>
+        <v>0.00010454</v>
       </c>
       <c r="R8">
-        <v>934250000</v>
+        <v>0.00017982</v>
       </c>
       <c r="S8">
-        <v>2449000000</v>
+        <v>0.00018491</v>
       </c>
       <c r="T8">
-        <v>4106100000</v>
+        <v>0.00018653</v>
       </c>
       <c r="U8">
-        <v>4841700000</v>
+        <v>0.00016712</v>
       </c>
       <c r="V8">
-        <v>4833500000</v>
+        <v>0.00014458</v>
       </c>
       <c r="W8">
-        <v>4264800000</v>
+        <v>0.00012603</v>
       </c>
       <c r="X8">
-        <v>3628100000</v>
+        <v>0.00011443</v>
       </c>
       <c r="Y8">
-        <v>3088100000</v>
+        <v>0.00011519</v>
       </c>
       <c r="Z8">
-        <v>2634100000</v>
+        <v>0.00011467</v>
       </c>
       <c r="AA8">
-        <v>2527200000</v>
+        <v>0.00010373</v>
       </c>
       <c r="AB8">
-        <v>2484900000</v>
+        <v>8.258399999999999E-05</v>
       </c>
       <c r="AC8">
-        <v>2177100000</v>
+        <v>7.425200000000001E-05</v>
       </c>
       <c r="AD8">
-        <v>1539500000</v>
+        <v>6.8965E-05</v>
       </c>
       <c r="AE8">
-        <v>1133300000</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>934250000</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <v>0</v>
@@ -1622,109 +1574,103 @@
       <c r="AR8">
         <v>0</v>
       </c>
-      <c r="AS8">
-        <v>0</v>
-      </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:44">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C9">
-        <v>64</v>
+        <v>9.077999999999999E-05</v>
       </c>
       <c r="D9">
-        <v>60</v>
+        <v>0.00015038</v>
       </c>
       <c r="E9">
-        <v>2087000000</v>
+        <v>0.00014553</v>
       </c>
       <c r="F9">
-        <v>3462600000</v>
+        <v>0.00013976</v>
       </c>
       <c r="G9">
-        <v>3984900000</v>
+        <v>0.0001165</v>
       </c>
       <c r="H9">
-        <v>3825900000</v>
+        <v>9.9035E-05</v>
       </c>
       <c r="I9">
-        <v>3259800000</v>
+        <v>8.496900000000001E-05</v>
       </c>
       <c r="J9">
-        <v>2793000000</v>
+        <v>7.655199999999999E-05</v>
       </c>
       <c r="K9">
-        <v>2247200000</v>
+        <v>7.9069E-05</v>
       </c>
       <c r="L9">
-        <v>1963800000</v>
+        <v>8.0856E-05</v>
       </c>
       <c r="M9">
-        <v>1999000000</v>
+        <v>7.1498E-05</v>
       </c>
       <c r="N9">
-        <v>1955600000</v>
+        <v>5.9916E-05</v>
       </c>
       <c r="O9">
-        <v>1742900000</v>
+        <v>5.7438E-05</v>
       </c>
       <c r="P9">
-        <v>1252600000</v>
+        <v>5.6889E-05</v>
       </c>
       <c r="Q9">
-        <v>1120000000</v>
+        <v>9.0781E-05</v>
       </c>
       <c r="R9">
-        <v>996250000</v>
+        <v>0.00015038</v>
       </c>
       <c r="S9">
-        <v>2087100000</v>
+        <v>0.00014553</v>
       </c>
       <c r="T9">
-        <v>3462600000</v>
+        <v>0.00013976</v>
       </c>
       <c r="U9">
-        <v>3984900000</v>
+        <v>0.0001165</v>
       </c>
       <c r="V9">
-        <v>3825700000</v>
+        <v>9.9035E-05</v>
       </c>
       <c r="W9">
-        <v>3259700000</v>
+        <v>8.496900000000001E-05</v>
       </c>
       <c r="X9">
-        <v>2793000000</v>
+        <v>7.6555E-05</v>
       </c>
       <c r="Y9">
-        <v>2247200000</v>
+        <v>7.9069E-05</v>
       </c>
       <c r="Z9">
-        <v>1963800000</v>
+        <v>8.085999999999999E-05</v>
       </c>
       <c r="AA9">
-        <v>1999500000</v>
+        <v>7.1498E-05</v>
       </c>
       <c r="AB9">
-        <v>1955600000</v>
+        <v>5.9901E-05</v>
       </c>
       <c r="AC9">
-        <v>1742900000</v>
+        <v>5.7438E-05</v>
       </c>
       <c r="AD9">
-        <v>1252600000</v>
+        <v>5.6889E-05</v>
       </c>
       <c r="AE9">
-        <v>1120000000</v>
+        <v>0</v>
       </c>
       <c r="AF9">
-        <v>995420000</v>
+        <v>0</v>
       </c>
       <c r="AG9">
         <v>0</v>
@@ -1762,109 +1708,103 @@
       <c r="AR9">
         <v>0</v>
       </c>
-      <c r="AS9">
-        <v>0</v>
-      </c>
-      <c r="AT9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:44">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C10">
-        <v>72</v>
+        <v>7.860399999999999E-05</v>
       </c>
       <c r="D10">
-        <v>68</v>
+        <v>0.00012549</v>
       </c>
       <c r="E10">
-        <v>1701700000</v>
+        <v>0.00011465</v>
       </c>
       <c r="F10">
-        <v>2923500000</v>
+        <v>0.00010466</v>
       </c>
       <c r="G10">
-        <v>3272900000</v>
+        <v>8.2597E-05</v>
       </c>
       <c r="H10">
-        <v>2913300000</v>
+        <v>6.928E-05</v>
       </c>
       <c r="I10">
-        <v>2556600000</v>
+        <v>5.7478E-05</v>
       </c>
       <c r="J10">
-        <v>2168300000</v>
+        <v>5.1575E-05</v>
       </c>
       <c r="K10">
-        <v>1813600000</v>
+        <v>5.4553E-05</v>
       </c>
       <c r="L10">
-        <v>1649600000</v>
+        <v>5.7346E-05</v>
       </c>
       <c r="M10">
-        <v>1671000000</v>
+        <v>5.1064E-05</v>
       </c>
       <c r="N10">
-        <v>1668200000</v>
+        <v>4.2572E-05</v>
       </c>
       <c r="O10">
-        <v>1443700000</v>
+        <v>4.5441E-05</v>
       </c>
       <c r="P10">
-        <v>1173400000</v>
+        <v>4.6959E-05</v>
       </c>
       <c r="Q10">
-        <v>1108600000</v>
+        <v>7.8601E-05</v>
       </c>
       <c r="R10">
-        <v>1025600000</v>
+        <v>0.00012549</v>
       </c>
       <c r="S10">
-        <v>1701700000</v>
+        <v>0.00011465</v>
       </c>
       <c r="T10">
-        <v>2923700000</v>
+        <v>0.00010466</v>
       </c>
       <c r="U10">
-        <v>3273000000</v>
+        <v>8.2599E-05</v>
       </c>
       <c r="V10">
-        <v>2913100000</v>
+        <v>6.928E-05</v>
       </c>
       <c r="W10">
-        <v>2556600000</v>
+        <v>5.7478E-05</v>
       </c>
       <c r="X10">
-        <v>2168300000</v>
+        <v>5.1568E-05</v>
       </c>
       <c r="Y10">
-        <v>1813600000</v>
+        <v>5.4553E-05</v>
       </c>
       <c r="Z10">
-        <v>1649600000</v>
+        <v>5.7346E-05</v>
       </c>
       <c r="AA10">
-        <v>1670500000</v>
+        <v>5.1064E-05</v>
       </c>
       <c r="AB10">
-        <v>1668200000</v>
+        <v>4.2572E-05</v>
       </c>
       <c r="AC10">
-        <v>1443700000</v>
+        <v>4.5441E-05</v>
       </c>
       <c r="AD10">
-        <v>1173400000</v>
+        <v>4.6959E-05</v>
       </c>
       <c r="AE10">
-        <v>1108600000</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <v>1025600000</v>
+        <v>0</v>
       </c>
       <c r="AG10">
         <v>0</v>
@@ -1902,109 +1842,103 @@
       <c r="AR10">
         <v>0</v>
       </c>
-      <c r="AS10">
-        <v>0</v>
-      </c>
-      <c r="AT10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:44">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>6.7615E-05</v>
       </c>
       <c r="D11">
-        <v>76</v>
+        <v>0.00010364</v>
       </c>
       <c r="E11">
-        <v>1351200000</v>
+        <v>8.9353E-05</v>
       </c>
       <c r="F11">
-        <v>2392400000</v>
+        <v>7.6548E-05</v>
       </c>
       <c r="G11">
-        <v>2570400000</v>
+        <v>5.852E-05</v>
       </c>
       <c r="H11">
-        <v>2214900000</v>
+        <v>4.7704E-05</v>
       </c>
       <c r="I11">
-        <v>2014300000</v>
+        <v>3.8821E-05</v>
       </c>
       <c r="J11">
-        <v>1653500000</v>
+        <v>3.5379E-05</v>
       </c>
       <c r="K11">
-        <v>1454000000</v>
+        <v>3.7667E-05</v>
       </c>
       <c r="L11">
-        <v>1354100000</v>
+        <v>3.9385E-05</v>
       </c>
       <c r="M11">
-        <v>1413800000</v>
+        <v>3.5143E-05</v>
       </c>
       <c r="N11">
-        <v>1349100000</v>
+        <v>3.0609E-05</v>
       </c>
       <c r="O11">
-        <v>1126900000</v>
+        <v>3.5375E-05</v>
       </c>
       <c r="P11">
-        <v>1058100000</v>
+        <v>3.8303E-05</v>
       </c>
       <c r="Q11">
-        <v>914890000</v>
+        <v>6.761399999999999E-05</v>
       </c>
       <c r="R11">
-        <v>723220000</v>
+        <v>0.00010364</v>
       </c>
       <c r="S11">
-        <v>1351200000</v>
+        <v>8.935700000000001E-05</v>
       </c>
       <c r="T11">
-        <v>2392200000</v>
+        <v>7.6543E-05</v>
       </c>
       <c r="U11">
-        <v>2570100000</v>
+        <v>5.8516E-05</v>
       </c>
       <c r="V11">
-        <v>2214900000</v>
+        <v>4.7706E-05</v>
       </c>
       <c r="W11">
-        <v>2014100000</v>
+        <v>3.8821E-05</v>
       </c>
       <c r="X11">
-        <v>1653500000</v>
+        <v>3.5379E-05</v>
       </c>
       <c r="Y11">
-        <v>1454000000</v>
+        <v>3.7667E-05</v>
       </c>
       <c r="Z11">
-        <v>1354100000</v>
+        <v>3.9385E-05</v>
       </c>
       <c r="AA11">
-        <v>1413800000</v>
+        <v>3.5139E-05</v>
       </c>
       <c r="AB11">
-        <v>1349100000</v>
+        <v>3.0609E-05</v>
       </c>
       <c r="AC11">
-        <v>1126900000</v>
+        <v>3.5375E-05</v>
       </c>
       <c r="AD11">
-        <v>1058100000</v>
+        <v>3.8303E-05</v>
       </c>
       <c r="AE11">
-        <v>914210000</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <v>723220000</v>
+        <v>0</v>
       </c>
       <c r="AG11">
         <v>0</v>
@@ -2040,12 +1974,6 @@
         <v>0</v>
       </c>
       <c r="AR11">
-        <v>0</v>
-      </c>
-      <c r="AS11">
-        <v>0</v>
-      </c>
-      <c r="AT11">
         <v>0</v>
       </c>
     </row>

</xml_diff>